<commit_message>
The work of the parser has been radically changed
</commit_message>
<xml_diff>
--- a/src/main/resources/sample.xlsx
+++ b/src/main/resources/sample.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Defalt\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyData\Programming\Java\FilesConverterAlfaBank\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BB67F64-9A3A-437B-B213-3C2031649C62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2EF9383-DD99-47B2-8A4F-3C9E7AA11772}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -126,7 +126,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -136,6 +136,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -156,9 +162,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="22" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="22" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -442,7 +448,7 @@
   <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -459,7 +465,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -539,7 +545,7 @@
       <c r="J2" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="3">
+      <c r="K2" s="5">
         <v>44734.388888888891</v>
       </c>
       <c r="L2" s="2">
@@ -554,7 +560,7 @@
       <c r="O2" s="1">
         <v>44734</v>
       </c>
-      <c r="P2" s="5">
+      <c r="P2" s="4">
         <v>0.3888888888888889</v>
       </c>
     </row>

</xml_diff>